<commit_message>
Defined false pos and false neg
Now need to work on percentages
</commit_message>
<xml_diff>
--- a/a good hard look.xlsx
+++ b/a good hard look.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>acute</t>
   </si>
@@ -42,13 +42,25 @@
     <t>Accuracy</t>
   </si>
   <si>
-    <t>True positives</t>
+    <t>trueneg</t>
   </si>
   <si>
-    <t>trueNeg</t>
+    <t>falseneg</t>
   </si>
   <si>
-    <t>True negatives</t>
+    <t>falsepos</t>
+  </si>
+  <si>
+    <t>Actual Yes</t>
+  </si>
+  <si>
+    <t>Actual No</t>
+  </si>
+  <si>
+    <t>Said Yes</t>
+  </si>
+  <si>
+    <t>Said No</t>
   </si>
 </sst>
 </file>
@@ -390,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A49" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -401,15 +413,12 @@
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
@@ -417,938 +426,1271 @@
       <c r="H1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8">
         <v>0</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0</v>
       </c>
       <c r="B10">
         <v>0</v>
       </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
       <c r="G16">
         <v>0</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
       <c r="G17">
         <v>1</v>
       </c>
       <c r="H17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
       <c r="G20">
         <v>1</v>
       </c>
       <c r="H20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
       <c r="G21">
         <v>0</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
       <c r="G22">
         <v>0</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
       <c r="G23">
         <v>1</v>
       </c>
       <c r="H23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
       <c r="G24">
         <v>1</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
       <c r="G26">
         <v>1</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
       <c r="G27">
         <v>1</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>0</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0</v>
       </c>
       <c r="B29">
         <v>0</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
       <c r="G29">
         <v>1</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>0</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
       <c r="G34">
         <v>1</v>
       </c>
       <c r="H34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
       <c r="G35">
         <v>1</v>
       </c>
       <c r="H35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38">
-        <v>0</v>
-      </c>
       <c r="G38">
         <v>1</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
       <c r="G39">
         <v>1</v>
       </c>
       <c r="H39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40">
-        <v>0</v>
-      </c>
       <c r="G40">
         <v>1</v>
       </c>
       <c r="H40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
-      <c r="C42">
-        <v>0</v>
-      </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>0</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
       <c r="G44">
         <v>1</v>
       </c>
       <c r="H44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
       <c r="G45">
         <v>1</v>
       </c>
       <c r="H45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
       <c r="G46">
         <v>0</v>
       </c>
       <c r="H46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
-      <c r="C47">
-        <v>0</v>
-      </c>
       <c r="G47">
         <v>1</v>
       </c>
       <c r="H47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
       <c r="G48">
         <v>0</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49">
-        <v>0</v>
-      </c>
       <c r="G49">
         <v>1</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
-      <c r="C50">
-        <v>1</v>
-      </c>
       <c r="G50">
         <v>1</v>
       </c>
       <c r="H50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
-      <c r="C51">
-        <v>1</v>
-      </c>
       <c r="G51">
         <v>1</v>
       </c>
       <c r="H51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1</v>
       </c>
       <c r="B52">
         <v>1</v>
       </c>
-      <c r="C52">
-        <v>0</v>
-      </c>
       <c r="G52">
         <v>1</v>
       </c>
       <c r="H52">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
-      <c r="C53">
-        <v>0</v>
-      </c>
       <c r="G53">
         <v>0</v>
       </c>
       <c r="H53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1</v>
       </c>
       <c r="B54">
         <v>1</v>
       </c>
-      <c r="C54">
-        <v>0</v>
-      </c>
       <c r="G54">
         <v>1</v>
       </c>
       <c r="H54">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
-      <c r="C55">
-        <v>0</v>
-      </c>
       <c r="G55">
         <v>1</v>
       </c>
       <c r="H55">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="1"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
@@ -1361,15 +1703,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1402,23 +1745,45 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <f>SUM(Data!H2:H55)</f>
         <v>27</v>
       </c>
+      <c r="C6">
+        <f>SUM(Data!K2:K55)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <f>SUM(Data!C2:C55)</f>
+        <f>SUM(Data!J2:J55)</f>
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f>SUM(Data!I2:I55)</f>
         <v>15</v>
       </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Calculated sensitivity and and specificity
</commit_message>
<xml_diff>
--- a/a good hard look.xlsx
+++ b/a good hard look.xlsx
@@ -16,15 +16,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>acute</t>
   </si>
   <si>
     <t>classifiedAs</t>
-  </si>
-  <si>
-    <t>confusion</t>
   </si>
   <si>
     <t>truepos</t>
@@ -62,12 +59,31 @@
   <si>
     <t>Said No</t>
   </si>
+  <si>
+    <t>agreements</t>
+  </si>
+  <si>
+    <t>Sensitivity</t>
+  </si>
+  <si>
+    <t>Totals</t>
+  </si>
+  <si>
+    <t>Specificity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,7 +100,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -92,18 +108,117 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -404,13 +519,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -421,19 +537,19 @@
         <v>1</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
       <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1703,10 +1819,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,75 +1831,113 @@
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <f>SUM(Data!G2:G55)</f>
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <f>54</f>
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="12">
         <f>B1/B2</f>
         <v>0.77777777777777779</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <f>SUM(Data!H2:H55)</f>
         <v>27</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="7">
         <f>SUM(Data!K2:K55)</f>
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
+      <c r="D6">
+        <f>SUM(B6:C6)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="9">
         <f>SUM(Data!J2:J55)</f>
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="10">
         <f>SUM(Data!I2:I55)</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>SUM(B7:C7)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>SUM(B6:B7)</f>
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <f>SUM(C6:C7)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="12">
+        <f>B6/B8</f>
+        <v>0.87096774193548387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="12">
+        <f>C7/C8</f>
+        <v>0.65217391304347827</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Calculated PPV and NPV
</commit_message>
<xml_diff>
--- a/a good hard look.xlsx
+++ b/a good hard look.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>acute</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Specificity</t>
+  </si>
+  <si>
+    <t>PPV</t>
+  </si>
+  <si>
+    <t>NPV</t>
   </si>
 </sst>
 </file>
@@ -198,7 +204,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -215,6 +220,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1819,15 +1827,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1853,7 +1861,7 @@
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <f>B1/B2</f>
         <v>0.77777777777777779</v>
       </c>
@@ -1862,11 +1870,11 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" t="s">
@@ -1874,14 +1882,14 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <f>SUM(Data!H2:H55)</f>
         <v>27</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <f>SUM(Data!K2:K55)</f>
         <v>8</v>
       </c>
@@ -1891,14 +1899,14 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <f>SUM(Data!J2:J55)</f>
         <v>4</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="9">
         <f>SUM(Data!I2:I55)</f>
         <v>15</v>
       </c>
@@ -1908,7 +1916,6 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
       <c r="B8">
         <f>SUM(B6:B7)</f>
         <v>31</v>
@@ -1918,25 +1925,40 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <f>B6/B8</f>
         <v>0.87096774193548387</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <f>C7/C8</f>
         <v>0.65217391304347827</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="11">
+        <f>B6/D6</f>
+        <v>0.77142857142857146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="11">
+        <f>C7/D7</f>
+        <v>0.78947368421052633</v>
       </c>
     </row>
   </sheetData>

</xml_diff>